<commit_message>
Further cleaning of script
added some comments and re-arranged code in a way that made a bit more
sense
</commit_message>
<xml_diff>
--- a/analyzed.xlsx
+++ b/analyzed.xlsx
@@ -359,121 +359,121 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="n">
-        <v>454.8362488205597</v>
+        <v>454.8362488205599</v>
       </c>
       <c r="B1" t="n">
-        <v>243.5906663222287</v>
+        <v>243.5906663222289</v>
       </c>
       <c r="C1" t="n">
         <v>64.09787188629774</v>
       </c>
       <c r="D1" t="n">
-        <v>15553.15128990203</v>
+        <v>15553.15128990207</v>
       </c>
       <c r="E1" t="n">
-        <v>19858.71060968669</v>
+        <v>19858.71060968659</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="n">
-        <v>424.9247425510384</v>
+        <v>424.9247425510387</v>
       </c>
       <c r="B2" t="n">
-        <v>148.5215430128698</v>
+        <v>148.5215430128691</v>
       </c>
       <c r="C2" t="n">
         <v>58.45243368568961</v>
       </c>
       <c r="D2" t="n">
-        <v>20618.76807637279</v>
+        <v>20618.76807637289</v>
       </c>
       <c r="E2" t="n">
-        <v>23889.29985000945</v>
+        <v>23889.29985000936</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="n">
-        <v>491.9968235684233</v>
+        <v>491.9968235684238</v>
       </c>
       <c r="B3" t="n">
         <v>262.3759591010767</v>
       </c>
       <c r="C3" t="n">
-        <v>50.82714781632767</v>
+        <v>50.82714781632766</v>
       </c>
       <c r="D3" t="n">
-        <v>17158.88839632446</v>
+        <v>17158.88839632451</v>
       </c>
       <c r="E3" t="n">
-        <v>21987.75490215387</v>
+        <v>21987.75490215343</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="n">
-        <v>427.8930531860109</v>
+        <v>427.8930531860114</v>
       </c>
       <c r="B4" t="n">
-        <v>149.4657574646344</v>
+        <v>149.4657574646348</v>
       </c>
       <c r="C4" t="n">
         <v>74.02632631701077</v>
       </c>
       <c r="D4" t="n">
-        <v>19888.17829793947</v>
+        <v>19888.17829793953</v>
       </c>
       <c r="E4" t="n">
-        <v>24815.62369374783</v>
+        <v>24815.62369374784</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="n">
-        <v>423.9592853753156</v>
+        <v>423.9592853753159</v>
       </c>
       <c r="B5" t="n">
-        <v>177.3435406178075</v>
+        <v>177.3435406178074</v>
       </c>
       <c r="C5" t="n">
-        <v>71.32600195071166</v>
+        <v>71.32600195071163</v>
       </c>
       <c r="D5" t="n">
-        <v>17937.59616870337</v>
+        <v>17937.59616870345</v>
       </c>
       <c r="E5" t="n">
-        <v>25748.67199864936</v>
+        <v>25748.67199864926</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="n">
-        <v>424.5737416353534</v>
+        <v>424.5737416353535</v>
       </c>
       <c r="B6" t="n">
         <v>150.0956755700667</v>
       </c>
       <c r="C6" t="n">
-        <v>70.40506668812043</v>
+        <v>70.40506668812024</v>
       </c>
       <c r="D6" t="n">
-        <v>20070.19309186738</v>
+        <v>20070.19309186744</v>
       </c>
       <c r="E6" t="n">
-        <v>29458.55043952705</v>
+        <v>29458.55043952695</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="n">
-        <v>441.3639825227837</v>
+        <v>441.3639825227841</v>
       </c>
       <c r="B7" t="n">
-        <v>191.1007915737026</v>
+        <v>191.1007915737025</v>
       </c>
       <c r="C7" t="n">
         <v>63.92147395772711</v>
       </c>
       <c r="D7" t="n">
-        <v>18537.79588685158</v>
+        <v>18537.79588685166</v>
       </c>
       <c r="E7" t="n">
-        <v>24293.10191562885</v>
+        <v>24293.10191562903</v>
       </c>
     </row>
   </sheetData>

</xml_diff>